<commit_message>
Added license disclaimer to every source file
Implemented an update thread, not working stable as it freezes once the first non payment message pops in
Changed flags field to hold payment success
still lot of development to go
</commit_message>
<xml_diff>
--- a/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
+++ b/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
@@ -117,9 +117,6 @@
     <t>Eg.: 79.76576,801.2764,15.16314</t>
   </si>
   <si>
-    <t>Eg.: 101</t>
-  </si>
-  <si>
     <t>Total current staff</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Game capital required to change owned flag to true</t>
   </si>
   <si>
-    <t>Unsed when flag is already true</t>
-  </si>
-  <si>
     <t>Showroom</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>Salary paid to every staff member before income calculation</t>
   </si>
   <si>
-    <t>If player can't met StaffSal * Staff, no income is calculated</t>
-  </si>
-  <si>
     <t>Up front payment to hire a new staff member</t>
   </si>
   <si>
@@ -213,7 +204,16 @@
     <t>LEAVE AT 0</t>
   </si>
   <si>
-    <t>Used as 'bulk storage' for the boolean variables [Ownable][Owned][ContextMission][ShowBlip]</t>
+    <t>Used as 'bulk storage' for the boolean variables [Ownable][Owned][ContextMission][StaffPayed]</t>
+  </si>
+  <si>
+    <t>Eg.: 1011</t>
+  </si>
+  <si>
+    <t>Unused when flag is already true</t>
+  </si>
+  <si>
+    <t>If player can't meet StaffSal * Staff, no income is calculated</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,21 +1000,21 @@
         <v>22</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="15"/>
       <c r="C10" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="15"/>
       <c r="C11" s="12" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,14 +1082,14 @@
         <v>25</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="12" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1107,10 +1107,10 @@
         <v>27</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,10 +1133,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,17 +1159,17 @@
         <v>27</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="15"/>
       <c r="C34" s="12" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1187,17 +1187,17 @@
         <v>27</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="15"/>
       <c r="C38" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1215,31 +1215,31 @@
         <v>27</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="15"/>
       <c r="C42" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="15"/>
       <c r="C43" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="24"/>
       <c r="C44" s="14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>26</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>20</v>
@@ -1309,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -1331,7 +1331,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -1342,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
@@ -1353,7 +1353,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
@@ -1364,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
@@ -1375,7 +1375,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
@@ -1386,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -1408,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
@@ -1441,7 +1441,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,25 +1476,25 @@
         <v>25</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1517,16 +1517,16 @@
         <v>599999</v>
       </c>
       <c r="G2" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H2" s="7">
-        <v>0</v>
+        <v>1500000</v>
       </c>
       <c r="I2" s="7">
-        <v>0</v>
+        <v>6500</v>
       </c>
       <c r="J2" s="7">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="K2" s="7">
         <v>0</v>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="M2" s="1" t="str">
         <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","&amp;L2&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','1011',0,10,599999,0, 0, 0, 0, 0,1);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','1011',0,10,599999,100, 1500000, 6500, 1500, 0,1);</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="4">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="M3" s="1" t="str">
         <f t="shared" ref="M3:M11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "','"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","&amp;L3&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','1002',0,10,399999,0, 0, 0, 0, 0,2);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','1001',0,10,399999,0, 0, 0, 0, 0,2);</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>